<commit_message>
Sostituzione file via upload
Sostituiti i file:

- CT3
- CT4
- data.json
- checklist accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUSXXX/Regione_Sardegna/PSWEB_SISaR_RAS/20.14/accreditamento-checklist_PSWEB_SISaR_RAS_V8.1.3.xlsx
+++ b/GATEWAY/A1#111DEDALUSXXX/Regione_Sardegna/PSWEB_SISaR_RAS/20.14/accreditamento-checklist_PSWEB_SISaR_RAS_V8.1.3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ACCREDITAMENTO\it-fse-accreditamento\GATEWAY\A1#111DEDALUSXXX\Regione_Sardegna\PSWEB_SISaR_RAS\20.14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toluf\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14A2272-8A4C-42E3-B067-EC1D5D8798FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC758B6-0B2F-4290-B29A-DFE8D1C7842B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="345" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,8 +22,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$383</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="oXWj5iU3LtnvLpdhFqszSz/X91q3fG5U5zC5TJKtiGw="/>
     </ext>
@@ -4584,6 +4593,15 @@
     <t>subject_application_version: 20.14</t>
   </si>
   <si>
+    <t>2023-11-03T11:09:23Z</t>
+  </si>
+  <si>
+    <t>e72ea2d810a0ab2c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.529091b0ed824e08be5d82e4b438bdf98c53c463382d335cbf038f185f5dd9ba.f96c7e53af^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
     <t>2023-10-11T22:57:15Z</t>
   </si>
   <si>
@@ -4890,31 +4908,22 @@
     <t>2.16.840.1.113883.2.9.2.200.4.4.d5809fea07b5089ca11bc401066533b5fc7493697ce980565d394420a194dac5.fb05f4c013^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-11-28T10:22:10Z</t>
-  </si>
-  <si>
-    <t>21805023c3289097</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.7264e468d7adad95d92027b5958f617448f97b4882d46c97c98308e4e57af9b4.1f8afe2e8e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-11-28T10:29:26Z</t>
-  </si>
-  <si>
-    <t>d9d488bd7166e3c6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.cac285cd993e6989a5266be26719f049a72678a9621262888b4ad7f7b1ef1c64.d3cd5091da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-11-24T17:11:58Z</t>
-  </si>
-  <si>
-    <t>f2f1268e638e8cac</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.7efc9af8444ee42ea570d6d4f70994a10de15e8d79b8c704230c9fd64f58ce03.2f7fe4b5a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>18b0b58942239b59</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.ec9fbeb1b4679f4a64a2668c91666c8d9221723fff10dc2dd5c30bf46b8e222b.4b801c58c9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-01T09:15:29Z</t>
+  </si>
+  <si>
+    <t>2023-12-01T09:13:46Z</t>
+  </si>
+  <si>
+    <t>7fb9afe1a07a4927</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.9aaf097d7a95772b138a8e180dd096091a7b9f7727524cf1a7f5191606e450f0.1ff8ee5532^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -7836,10 +7845,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
+      <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -8825,16 +8834,16 @@
         <v>95</v>
       </c>
       <c r="F31" s="20">
-        <v>45254</v>
+        <v>45233</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>960</v>
+        <v>852</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>961</v>
+        <v>853</v>
       </c>
       <c r="I31" s="21" t="s">
-        <v>962</v>
+        <v>854</v>
       </c>
       <c r="J31" s="22" t="s">
         <v>139</v>
@@ -8872,13 +8881,13 @@
         <v>45258</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>951</v>
+        <v>954</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>952</v>
+        <v>955</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>953</v>
+        <v>956</v>
       </c>
       <c r="J32" s="22" t="s">
         <v>139</v>
@@ -8913,16 +8922,16 @@
         <v>99</v>
       </c>
       <c r="F33" s="20">
-        <v>45258</v>
+        <v>45261</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>954</v>
+        <v>960</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="J33" s="22" t="s">
         <v>139</v>
@@ -8957,16 +8966,16 @@
         <v>101</v>
       </c>
       <c r="F34" s="20">
-        <v>45258</v>
+        <v>45261</v>
       </c>
       <c r="G34" s="21" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>958</v>
+        <v>961</v>
       </c>
       <c r="I34" s="21" t="s">
-        <v>959</v>
+        <v>962</v>
       </c>
       <c r="J34" s="22" t="s">
         <v>139</v>
@@ -9242,13 +9251,13 @@
         <v>45236</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>857</v>
+        <v>860</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="J42" s="22" t="s">
         <v>139</v>
@@ -9265,7 +9274,7 @@
         <v>139</v>
       </c>
       <c r="P42" s="36" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="Q42" s="22"/>
       <c r="R42" s="23"/>
@@ -9532,13 +9541,13 @@
         <v>45236</v>
       </c>
       <c r="G50" s="21" t="s">
+        <v>861</v>
+      </c>
+      <c r="H50" s="21" t="s">
+        <v>862</v>
+      </c>
+      <c r="I50" s="21" t="s">
         <v>858</v>
-      </c>
-      <c r="H50" s="21" t="s">
-        <v>859</v>
-      </c>
-      <c r="I50" s="21" t="s">
-        <v>855</v>
       </c>
       <c r="J50" s="22" t="s">
         <v>139</v>
@@ -9555,7 +9564,7 @@
         <v>139</v>
       </c>
       <c r="P50" s="36" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="Q50" s="22"/>
       <c r="R50" s="23"/>
@@ -9597,7 +9606,7 @@
         <v>139</v>
       </c>
       <c r="P51" s="36" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="Q51" s="22"/>
       <c r="R51" s="23" t="s">
@@ -9861,7 +9870,7 @@
         <v>139</v>
       </c>
       <c r="P58" s="36" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="Q58" s="22"/>
       <c r="R58" s="23" t="s">
@@ -12272,13 +12281,13 @@
         <v>45236</v>
       </c>
       <c r="G129" s="21" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c r="H129" s="21" t="s">
-        <v>861</v>
+        <v>864</v>
       </c>
       <c r="I129" s="21" t="s">
-        <v>862</v>
+        <v>865</v>
       </c>
       <c r="J129" s="22" t="s">
         <v>139</v>
@@ -12295,7 +12304,7 @@
         <v>139</v>
       </c>
       <c r="P129" s="22" t="s">
-        <v>937</v>
+        <v>940</v>
       </c>
       <c r="Q129" s="22"/>
       <c r="R129" s="23"/>
@@ -12324,13 +12333,13 @@
         <v>45236</v>
       </c>
       <c r="G130" s="21" t="s">
-        <v>863</v>
+        <v>866</v>
       </c>
       <c r="H130" s="21" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
       <c r="I130" s="21" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="J130" s="22" t="s">
         <v>139</v>
@@ -12343,13 +12352,13 @@
         <v>139</v>
       </c>
       <c r="N130" s="22" t="s">
-        <v>938</v>
+        <v>941</v>
       </c>
       <c r="O130" s="22" t="s">
         <v>848</v>
       </c>
       <c r="P130" s="22" t="s">
-        <v>939</v>
+        <v>942</v>
       </c>
       <c r="Q130" s="22"/>
       <c r="R130" s="23"/>
@@ -12378,13 +12387,13 @@
         <v>45236</v>
       </c>
       <c r="G131" s="21" t="s">
-        <v>866</v>
+        <v>869</v>
       </c>
       <c r="H131" s="21" t="s">
-        <v>867</v>
+        <v>870</v>
       </c>
       <c r="I131" s="21" t="s">
-        <v>868</v>
+        <v>871</v>
       </c>
       <c r="J131" s="22" t="s">
         <v>139</v>
@@ -12401,7 +12410,7 @@
         <v>139</v>
       </c>
       <c r="P131" s="22" t="s">
-        <v>940</v>
+        <v>943</v>
       </c>
       <c r="Q131" s="22"/>
       <c r="R131" s="23"/>
@@ -12430,13 +12439,13 @@
         <v>45236</v>
       </c>
       <c r="G132" s="21" t="s">
-        <v>869</v>
+        <v>872</v>
       </c>
       <c r="H132" s="21" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c r="I132" s="21" t="s">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c r="J132" s="22" t="s">
         <v>139</v>
@@ -12449,13 +12458,13 @@
         <v>139</v>
       </c>
       <c r="N132" s="22" t="s">
-        <v>941</v>
+        <v>944</v>
       </c>
       <c r="O132" s="22" t="s">
         <v>848</v>
       </c>
       <c r="P132" s="22" t="s">
-        <v>942</v>
+        <v>945</v>
       </c>
       <c r="Q132" s="22"/>
       <c r="R132" s="23"/>
@@ -12484,13 +12493,13 @@
         <v>45236</v>
       </c>
       <c r="G133" s="21" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c r="H133" s="21" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c r="I133" s="21" t="s">
-        <v>874</v>
+        <v>877</v>
       </c>
       <c r="J133" s="22" t="s">
         <v>139</v>
@@ -12503,13 +12512,13 @@
         <v>139</v>
       </c>
       <c r="N133" s="22" t="s">
-        <v>943</v>
+        <v>946</v>
       </c>
       <c r="O133" s="22" t="s">
         <v>848</v>
       </c>
       <c r="P133" s="22" t="s">
-        <v>942</v>
+        <v>945</v>
       </c>
       <c r="Q133" s="22"/>
       <c r="R133" s="23"/>
@@ -12538,13 +12547,13 @@
         <v>45236</v>
       </c>
       <c r="G134" s="21" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="H134" s="21" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="I134" s="21" t="s">
-        <v>877</v>
+        <v>880</v>
       </c>
       <c r="J134" s="22" t="s">
         <v>139</v>
@@ -12561,7 +12570,7 @@
         <v>848</v>
       </c>
       <c r="P134" s="22" t="s">
-        <v>944</v>
+        <v>947</v>
       </c>
       <c r="Q134" s="22"/>
       <c r="R134" s="23"/>
@@ -12590,13 +12599,13 @@
         <v>45237</v>
       </c>
       <c r="G135" s="21" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c r="H135" s="21" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c r="I135" s="21" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c r="J135" s="22" t="s">
         <v>139</v>
@@ -12609,13 +12618,13 @@
         <v>139</v>
       </c>
       <c r="N135" s="22" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c r="O135" s="22" t="s">
         <v>848</v>
       </c>
       <c r="P135" s="22" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="Q135" s="22"/>
       <c r="R135" s="23"/>
@@ -12644,13 +12653,13 @@
         <v>45237</v>
       </c>
       <c r="G136" s="21" t="s">
-        <v>881</v>
+        <v>884</v>
       </c>
       <c r="H136" s="21" t="s">
-        <v>882</v>
+        <v>885</v>
       </c>
       <c r="I136" s="21" t="s">
-        <v>883</v>
+        <v>886</v>
       </c>
       <c r="J136" s="22" t="s">
         <v>139</v>
@@ -12667,7 +12676,7 @@
         <v>848</v>
       </c>
       <c r="P136" s="22" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="Q136" s="22"/>
       <c r="R136" s="23"/>
@@ -12696,13 +12705,13 @@
         <v>45237</v>
       </c>
       <c r="G137" s="21" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c r="H137" s="21" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="I137" s="21" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
       <c r="J137" s="22" t="s">
         <v>139</v>
@@ -12715,13 +12724,13 @@
         <v>139</v>
       </c>
       <c r="N137" s="22" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c r="O137" s="22" t="s">
         <v>848</v>
       </c>
       <c r="P137" s="22" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="Q137" s="22"/>
       <c r="R137" s="23"/>
@@ -12750,13 +12759,13 @@
         <v>45237</v>
       </c>
       <c r="G138" s="21" t="s">
-        <v>889</v>
+        <v>892</v>
       </c>
       <c r="H138" s="21" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
       <c r="I138" s="21" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="J138" s="22" t="s">
         <v>139</v>
@@ -12769,13 +12778,13 @@
         <v>139</v>
       </c>
       <c r="N138" s="22" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c r="O138" s="22" t="s">
         <v>848</v>
       </c>
       <c r="P138" s="22" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="Q138" s="22"/>
       <c r="R138" s="23"/>
@@ -12804,13 +12813,13 @@
         <v>45237</v>
       </c>
       <c r="G139" s="21" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c r="H139" s="21" t="s">
-        <v>891</v>
+        <v>894</v>
       </c>
       <c r="I139" s="21" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
       <c r="J139" s="22" t="s">
         <v>139</v>
@@ -12823,13 +12832,13 @@
         <v>139</v>
       </c>
       <c r="N139" s="22" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c r="O139" s="22" t="s">
         <v>848</v>
       </c>
       <c r="P139" s="22" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="Q139" s="22"/>
       <c r="R139" s="23"/>
@@ -12858,13 +12867,13 @@
         <v>45237</v>
       </c>
       <c r="G140" s="21" t="s">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c r="H140" s="21" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c r="I140" s="21" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c r="J140" s="22" t="s">
         <v>139</v>
@@ -12877,13 +12886,13 @@
         <v>139</v>
       </c>
       <c r="N140" s="22" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="O140" s="22" t="s">
         <v>848</v>
       </c>
       <c r="P140" s="22" t="s">
-        <v>948</v>
+        <v>951</v>
       </c>
       <c r="Q140" s="22"/>
       <c r="R140" s="23"/>
@@ -12912,13 +12921,13 @@
         <v>45237</v>
       </c>
       <c r="G141" s="21" t="s">
-        <v>896</v>
+        <v>899</v>
       </c>
       <c r="H141" s="21" t="s">
-        <v>897</v>
+        <v>900</v>
       </c>
       <c r="I141" s="21" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="J141" s="22" t="s">
         <v>139</v>
@@ -12935,7 +12944,7 @@
         <v>139</v>
       </c>
       <c r="P141" s="36" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="Q141" s="22"/>
       <c r="R141" s="23"/>
@@ -12964,13 +12973,13 @@
         <v>45237</v>
       </c>
       <c r="G142" s="21" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c r="H142" s="21" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="I142" s="21" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="J142" s="22" t="s">
         <v>139</v>
@@ -12987,7 +12996,7 @@
         <v>139</v>
       </c>
       <c r="P142" s="36" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="Q142" s="22"/>
       <c r="R142" s="23"/>
@@ -13016,13 +13025,13 @@
         <v>45237</v>
       </c>
       <c r="G143" s="21" t="s">
-        <v>902</v>
+        <v>905</v>
       </c>
       <c r="H143" s="21" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="I143" s="21" t="s">
-        <v>904</v>
+        <v>907</v>
       </c>
       <c r="J143" s="22" t="s">
         <v>139</v>
@@ -13039,7 +13048,7 @@
         <v>139</v>
       </c>
       <c r="P143" s="36" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="Q143" s="22"/>
       <c r="R143" s="23"/>
@@ -13068,13 +13077,13 @@
         <v>45237</v>
       </c>
       <c r="G144" s="21" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="H144" s="21" t="s">
-        <v>906</v>
+        <v>909</v>
       </c>
       <c r="I144" s="21" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="J144" s="22" t="s">
         <v>139</v>
@@ -13087,13 +13096,13 @@
         <v>139</v>
       </c>
       <c r="N144" s="22" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c r="O144" s="22" t="s">
         <v>848</v>
       </c>
       <c r="P144" s="22" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="Q144" s="22"/>
       <c r="R144" s="23"/>
@@ -13122,13 +13131,13 @@
         <v>45237</v>
       </c>
       <c r="G145" s="21" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="H145" s="21" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="I145" s="21" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="J145" s="22" t="s">
         <v>139</v>
@@ -13145,7 +13154,7 @@
         <v>139</v>
       </c>
       <c r="P145" s="36" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="Q145" s="22"/>
       <c r="R145" s="23"/>
@@ -13174,13 +13183,13 @@
         <v>45237</v>
       </c>
       <c r="G146" s="21" t="s">
-        <v>911</v>
+        <v>914</v>
       </c>
       <c r="H146" s="21" t="s">
-        <v>912</v>
+        <v>915</v>
       </c>
       <c r="I146" s="21" t="s">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="J146" s="22" t="s">
         <v>139</v>
@@ -13197,7 +13206,7 @@
         <v>848</v>
       </c>
       <c r="P146" s="22" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="Q146" s="22"/>
       <c r="R146" s="23"/>
@@ -13226,13 +13235,13 @@
         <v>45237</v>
       </c>
       <c r="G147" s="21" t="s">
-        <v>914</v>
+        <v>917</v>
       </c>
       <c r="H147" s="21" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="I147" s="21" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
       <c r="J147" s="22" t="s">
         <v>139</v>
@@ -13245,13 +13254,13 @@
         <v>139</v>
       </c>
       <c r="N147" s="22" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c r="O147" s="22" t="s">
         <v>848</v>
       </c>
       <c r="P147" s="22" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="Q147" s="22"/>
       <c r="R147" s="23"/>
@@ -13280,13 +13289,13 @@
         <v>45237</v>
       </c>
       <c r="G148" s="21" t="s">
-        <v>917</v>
+        <v>920</v>
       </c>
       <c r="H148" s="21" t="s">
-        <v>918</v>
+        <v>921</v>
       </c>
       <c r="I148" s="21" t="s">
-        <v>919</v>
+        <v>922</v>
       </c>
       <c r="J148" s="22" t="s">
         <v>139</v>
@@ -13299,13 +13308,13 @@
         <v>139</v>
       </c>
       <c r="N148" s="22" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c r="O148" s="22" t="s">
         <v>848</v>
       </c>
       <c r="P148" s="22" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="Q148" s="22"/>
       <c r="R148" s="23"/>
@@ -13334,13 +13343,13 @@
         <v>45237</v>
       </c>
       <c r="G149" s="21" t="s">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="H149" s="21" t="s">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="I149" s="21" t="s">
-        <v>922</v>
+        <v>925</v>
       </c>
       <c r="J149" s="22" t="s">
         <v>139</v>
@@ -13357,7 +13366,7 @@
         <v>848</v>
       </c>
       <c r="P149" s="22" t="s">
-        <v>950</v>
+        <v>953</v>
       </c>
       <c r="Q149" s="22"/>
       <c r="R149" s="23"/>
@@ -13386,13 +13395,13 @@
         <v>45237</v>
       </c>
       <c r="G150" s="37" t="s">
-        <v>924</v>
+        <v>927</v>
       </c>
       <c r="H150" s="21" t="s">
-        <v>923</v>
+        <v>926</v>
       </c>
       <c r="I150" s="21" t="s">
-        <v>925</v>
+        <v>928</v>
       </c>
       <c r="J150" s="22" t="s">
         <v>139</v>
@@ -13409,7 +13418,7 @@
         <v>848</v>
       </c>
       <c r="P150" s="22" t="s">
-        <v>950</v>
+        <v>953</v>
       </c>
       <c r="Q150" s="22"/>
       <c r="R150" s="23"/>
@@ -13438,13 +13447,13 @@
         <v>45237</v>
       </c>
       <c r="G151" s="21" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="H151" s="21" t="s">
-        <v>927</v>
+        <v>930</v>
       </c>
       <c r="I151" s="21" t="s">
-        <v>928</v>
+        <v>931</v>
       </c>
       <c r="J151" s="22" t="s">
         <v>139</v>
@@ -13461,7 +13470,7 @@
         <v>848</v>
       </c>
       <c r="P151" s="22" t="s">
-        <v>950</v>
+        <v>953</v>
       </c>
       <c r="Q151" s="22"/>
       <c r="R151" s="23"/>
@@ -13490,13 +13499,13 @@
         <v>45237</v>
       </c>
       <c r="G152" s="21" t="s">
-        <v>929</v>
+        <v>932</v>
       </c>
       <c r="H152" s="21" t="s">
-        <v>930</v>
+        <v>933</v>
       </c>
       <c r="I152" s="21" t="s">
-        <v>931</v>
+        <v>934</v>
       </c>
       <c r="J152" s="22" t="s">
         <v>139</v>
@@ -13513,7 +13522,7 @@
         <v>848</v>
       </c>
       <c r="P152" s="22" t="s">
-        <v>950</v>
+        <v>953</v>
       </c>
       <c r="Q152" s="22"/>
       <c r="R152" s="23"/>
@@ -13542,13 +13551,13 @@
         <v>45237</v>
       </c>
       <c r="G153" s="21" t="s">
-        <v>932</v>
+        <v>935</v>
       </c>
       <c r="H153" s="21" t="s">
-        <v>933</v>
+        <v>936</v>
       </c>
       <c r="I153" s="21" t="s">
-        <v>934</v>
+        <v>937</v>
       </c>
       <c r="J153" s="22" t="s">
         <v>139</v>
@@ -13565,7 +13574,7 @@
         <v>139</v>
       </c>
       <c r="P153" s="36" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="Q153" s="22"/>
       <c r="R153" s="23"/>
@@ -21278,13 +21287,13 @@
         <v>45210</v>
       </c>
       <c r="G380" s="21" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c r="H380" s="21" t="s">
-        <v>853</v>
+        <v>856</v>
       </c>
       <c r="I380" s="21" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="J380" s="22" t="s">
         <v>139</v>

</xml_diff>